<commit_message>
Updated visual chart (new test with more controls)
</commit_message>
<xml_diff>
--- a/src/Visual/Visual Performance.xlsx
+++ b/src/Visual/Visual Performance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Documents\GitHub\xamarin-forms-perf-playground\src\Visual\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{030B57FF-0FBA-404B-A33C-E146BF94F9E2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AC9A41C-715A-4BD5-B391-CF1D3C2D1F42}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="3" tint="-0.24994659260841701"/>
@@ -103,6 +103,14 @@
       <name val="Trebuchet MS"/>
       <family val="2"/>
       <scheme val="major"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="3" tint="-0.24994659260841701"/>
+      <name val="Corbel"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -158,7 +166,7 @@
       <alignment horizontal="right"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -173,6 +181,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Components" xfId="5" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -372,10 +381,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>821</c:v>
+                  <c:v>612</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>919</c:v>
+                  <c:v>625</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1467,7 +1476,7 @@
   <dimension ref="B1:D6"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1504,9 +1513,9 @@
         <v>4</v>
       </c>
       <c r="C4" s="3">
-        <v>821</v>
+        <v>612</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="6">
         <v>154</v>
       </c>
     </row>
@@ -1515,7 +1524,7 @@
         <v>5</v>
       </c>
       <c r="C5" s="3">
-        <v>919</v>
+        <v>625</v>
       </c>
       <c r="D5" s="3">
         <v>169</v>

</xml_diff>